<commit_message>
Fix spelling in raw data.
</commit_message>
<xml_diff>
--- a/raw/Grand List Data revised 4-2017.xlsx
+++ b/raw/Grand List Data revised 4-2017.xlsx
@@ -6188,7 +6188,7 @@
     <t xml:space="preserve">LTD Properties LLC</t>
   </si>
   <si>
-    <t xml:space="preserve">LSC-Westminster Partnership</t>
+    <t xml:space="preserve">LCS-Westminster Partnership</t>
   </si>
   <si>
     <t xml:space="preserve">Aquarion Water</t>
@@ -6836,36 +6836,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.25"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="257" min="30" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="257" min="30" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22631,46 +22631,46 @@
   <dimension ref="A1:IW174"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D118" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D109" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A118" activeCellId="0" sqref="A118"/>
-      <selection pane="bottomRight" activeCell="G142" activeCellId="0" sqref="G142"/>
+      <selection pane="bottomLeft" activeCell="A109" activeCellId="0" sqref="A109"/>
+      <selection pane="bottomRight" activeCell="G148" activeCellId="0" sqref="G148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="59.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="9" width="44.9540816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="11" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="11" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="9" width="41.7142857142857"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="9" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="9" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="11" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="9" width="48.3265306122449"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="11" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="9" width="64.1224489795918"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="11" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="9" width="39.8214285714286"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="11" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="9" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="11" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="11" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="13" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="11" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="11" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="14" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="257" min="30" style="9" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="20.25"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="58.8571428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="9" width="44.4132653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="11" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="11" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="9" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="9" width="42.25"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="9" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="11" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="9" width="47.6530612244898"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="11" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="9" width="63.4438775510204"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="11" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="9" width="39.4183673469388"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="11" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="9" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="11" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="11" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="13" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="11" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="11" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="14" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="257" min="30" style="9" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>